<commit_message>
Updated SFI GM,VR and UF
</commit_message>
<xml_diff>
--- a/testData/SFI_AllMobilePopups_Tbl_RThree.xlsx
+++ b/testData/SFI_AllMobilePopups_Tbl_RThree.xlsx
@@ -11,7 +11,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t>BuildUrl</t>
   </si>
@@ -72,19 +72,29 @@
     <t>UF_Prefix</t>
   </si>
   <si>
-    <t>https://rthree.live/showform?formid=220136&amp;nurams=bot1</t>
-  </si>
-  <si>
     <t>SFAllMBPopups_Independent</t>
   </si>
   <si>
     <t>SFI_AllMobilePopups_Tbl_Rthree</t>
+  </si>
+  <si>
+    <t>https://rthree.live/showform?formid=829192&amp;nurams=bot1</t>
+  </si>
+  <si>
+    <t>voice_record_04112023</t>
+  </si>
+  <si>
+    <t>voice_record_06112023</t>
+  </si>
+  <si>
+    <t>formshow_06112023</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -130,9 +140,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -415,95 +424,101 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:AU2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="52.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="52.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="52.1796875"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="25.81640625"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="28.7265625"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="52.1796875"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="19.453125"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="21.1796875"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="28.26953125"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="20.7265625"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="13.6328125"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="18.54296875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" t="s" s="0">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" t="s" s="0">
         <v>14</v>
+      </c>
+      <c r="K2" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="AR2" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="AU2" t="s" s="0">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>